<commit_message>
Added 'Article' for Le/la/l'
</commit_message>
<xml_diff>
--- a/data/Characters.xlsx
+++ b/data/Characters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unice-my.sharepoint.com/personal/matis_herrmann_etu_unice_fr/Documents/Cours/S5/PS5/Citadelles/projet2-ps5-21-22-ps5-21-22-projet2-h/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="8_{EA873FCA-3AB6-4039-B52F-E8BC2F7155CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9E226C52-9B09-40E6-87AE-739006C131A0}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="8_{EA873FCA-3AB6-4039-B52F-E8BC2F7155CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{68AD6D61-4494-4288-A0F4-A14D72A4A54D}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{03545E87-65A1-4C32-966D-0B2F82E37BB4}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
   <si>
     <t>Id</t>
   </si>
@@ -60,9 +60,6 @@
     <t>Soldatesque</t>
   </si>
   <si>
-    <t>Assasin</t>
-  </si>
-  <si>
     <t>Voleur</t>
   </si>
   <si>
@@ -109,6 +106,21 @@
   </si>
   <si>
     <t>L'Architecte pioche deux cartes quartier en plus. il peut bâtir jusqu'à trois quartiers.</t>
+  </si>
+  <si>
+    <t>Assassin</t>
+  </si>
+  <si>
+    <t>Article</t>
+  </si>
+  <si>
+    <t>L'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Le </t>
+  </si>
+  <si>
+    <t xml:space="preserve">La </t>
   </si>
 </sst>
 </file>
@@ -466,10 +478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5458A47F-7758-463A-BF68-D15729B803E0}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -479,7 +491,7 @@
     <col min="4" max="4" width="159.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -492,117 +504,144 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E3" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ajout de choix de Personnage plus approfondi #50
</commit_message>
<xml_diff>
--- a/data/Characters.xlsx
+++ b/data/Characters.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -478,7 +478,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>